<commit_message>
update DQ report notes docs
</commit_message>
<xml_diff>
--- a/Scripts/Vacc HB DQ Summary template.xlsx
+++ b/Scripts/Vacc HB DQ Summary template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\nssstats01\VaccineDM\vacc_weekly_dq_reporting\Scripts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\stats\cl-out\michab06\vacc-dq-reporting\Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86A858C8-98FC-4C38-9763-BF986C3215D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F36F4AAE-F42D-4AD1-96D0-0E1D5EB226BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1204,17 +1204,201 @@
   </si>
   <si>
     <r>
-      <t>22. PNEUM Age &lt;2 years</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - Pneumococcal vaccination records where the patient is under 2 years old at vaccination. Based on column S - age_at_vacc which is calculated using column AC - patient_date_of_birth and column I - vacc_occurence_time.</t>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>23. All query data</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - All records that appear in the above queries. (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>QueryType</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is listed in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>column A</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">.) This can be used to focus on individual patients by filtering by </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>column D - patient_derived_upi_number</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, to see all data quality queries against them, rather than by query type.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Column AH - patient_nrs_date_of_death</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is included but, due to inconsistencies with this data in the VDL, should only be used in conjunction with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>column AG - patient_chi_derived_status_desc</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> for assurance on whether a person has died.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>06. COV Booster interval &lt; 12 weeks</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Covid-19 records where the patient has received a booster dose less than 12 weeks (84 days) after their previous vaccination.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>16. HZ Dose 2 interval &lt; 56 days</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Herpes zoster dose 2 records where the interval between dose 1 and dose 2 given is less than 56 days.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>01. Missing/Invalid CHI number</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Patients who have been recorded without a CHI number or with an invalid CHI number.</t>
     </r>
   </si>
   <si>
@@ -1229,206 +1413,64 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> - Herpes zoster vaccination records where, from 1st Sep 2023, the patient is not age 65 or 70-79 at 1st Sep 2023, or for previous years where a patient was not age 70-79 at the 1st Sep.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>23. All query data</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - All records that appear in the above queries. (</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>QueryType</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> is listed in </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>column A</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">.) This can be used to focus on individual patients by filtering by </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>column D - patient_derived_upi_number</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, to see all data quality queries against them, rather than by query type.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Column AH - patient_nrs_date_of_death</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> is included but, due to inconsistencies with this data in the VDL, should only be used in conjunction with </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>column AG - patient_chi_derived_status_desc</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> for assurance on whether a person has died.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>06. COV Booster interval &lt; 12 weeks</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - Covid-19 records where the patient has received a booster dose less than 12 weeks (84 days) after their previous vaccination.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>16. HZ Dose 2 interval &lt; 56 days</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - Herpes zoster dose 2 records where the interval between dose 1 and dose 2 given is less than 56 days.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>01. Missing/Invalid CHI number</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - Patients who have been recorded without a CHI number or with an invalid CHI number.</t>
+      <t xml:space="preserve"> - Herpes zoster vaccination records where, from 1st Sep 2023, the patient is not age 65 or 70-79 at 1st Sep 2023, or for previous years where a patient was not age 70-79 at the 1st Sep, and are not in an eligibility cohort.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>22. PNEUM Vacc given outwith age guidance</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Pneumococcal vaccination records where the patient is under 65 years old at vaccination and not in an other eligibility cohort. Based on column S - age_at_vacc which is calculated using </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">column AC - patient_date_of_birth </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>and</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> column I - vacc_occurence_time</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
     </r>
   </si>
 </sst>
@@ -1932,7 +1974,7 @@
   <dimension ref="B3:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1997,7 +2039,7 @@
       <c r="B9" s="1"/>
       <c r="C9" s="6"/>
       <c r="D9" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="1"/>
@@ -2031,7 +2073,7 @@
       <c r="B13" s="1"/>
       <c r="C13" s="6"/>
       <c r="D13" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="1"/>
@@ -2076,7 +2118,7 @@
       <c r="B18" s="1"/>
       <c r="C18" s="6"/>
       <c r="D18" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E18" s="7"/>
       <c r="F18" s="1"/>
@@ -2166,7 +2208,7 @@
       <c r="B28" s="1"/>
       <c r="C28" s="6"/>
       <c r="D28" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E28" s="7"/>
       <c r="F28" s="1"/>
@@ -2202,7 +2244,7 @@
       <c r="B32" s="1"/>
       <c r="C32" s="6"/>
       <c r="D32" s="17" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E32" s="7"/>
       <c r="F32" s="1"/>
@@ -2220,7 +2262,7 @@
       <c r="B34" s="1"/>
       <c r="C34" s="6"/>
       <c r="D34" s="17" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="E34" s="7"/>
       <c r="F34" s="1"/>
@@ -2229,7 +2271,7 @@
       <c r="B35" s="1"/>
       <c r="C35" s="6"/>
       <c r="D35" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E35" s="7"/>
       <c r="F35" s="1"/>

</xml_diff>

<commit_message>
In main script: add in save points for Event Summary, multi_vacc, covid_vacc & flu_vacc tables for restarts in case of Posit session crashing; add in RSV DQ report from separate script.
Update report summary notes to reflect addition of RSV in main script.
</commit_message>
<xml_diff>
--- a/Scripts/Vacc HB DQ Summary template.xlsx
+++ b/Scripts/Vacc HB DQ Summary template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\stats\cl-out\michab06\vacc-dq-reporting\Scripts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\nssstats01\VaccineDM\Mike\vacc-dq-reporting\Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F36F4AAE-F42D-4AD1-96D0-0E1D5EB226BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66F3756F-1739-42AF-B9B9-9856FB6D47CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
   <si>
     <t>Notes on the report:</t>
   </si>
@@ -1205,14 +1205,222 @@
   <si>
     <r>
       <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>23. All query data</t>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Column AH - patient_nrs_date_of_death</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is included but, due to inconsistencies with this data in the VDL, should only be used in conjunction with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>column AG - patient_chi_derived_status_desc</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> for assurance on whether a person has died.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>06. COV Booster interval &lt; 12 weeks</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Covid-19 records where the patient has received a booster dose less than 12 weeks (84 days) after their previous vaccination.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>16. HZ Dose 2 interval &lt; 56 days</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Herpes zoster dose 2 records where the interval between dose 1 and dose 2 given is less than 56 days.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>01. Missing/Invalid CHI number</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Patients who have been recorded without a CHI number or with an invalid CHI number.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>20. HZ Vacc given outwith age guidance</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Herpes zoster vaccination records where, from 1st Sep 2023, the patient is not age 65 or 70-79 at 1st Sep 2023, or for previous years where a patient was not age 70-79 at the 1st Sep, and are not in an eligibility cohort.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>22. PNEUM Vacc given outwith age guidance</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Pneumococcal vaccination records where the patient is under 65 years old at vaccination and not in an other eligibility cohort. Based on column S - age_at_vacc which is calculated using </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">column AC - patient_date_of_birth </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>and</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> column I - vacc_occurence_time</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>23. RSV Booster Recorded</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Records where a booster vaccination has been recorded.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>25. All query data</t>
     </r>
     <r>
       <rPr>
@@ -1291,186 +1499,24 @@
   <si>
     <r>
       <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Column AH - patient_nrs_date_of_death</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> is included but, due to inconsistencies with this data in the VDL, should only be used in conjunction with </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>column AG - patient_chi_derived_status_desc</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> for assurance on whether a person has died.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>06. COV Booster interval &lt; 12 weeks</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - Covid-19 records where the patient has received a booster dose less than 12 weeks (84 days) after their previous vaccination.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>16. HZ Dose 2 interval &lt; 56 days</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - Herpes zoster dose 2 records where the interval between dose 1 and dose 2 given is less than 56 days.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>01. Missing/Invalid CHI number</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - Patients who have been recorded without a CHI number or with an invalid CHI number.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>20. HZ Vacc given outwith age guidance</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - Herpes zoster vaccination records where, from 1st Sep 2023, the patient is not age 65 or 70-79 at 1st Sep 2023, or for previous years where a patient was not age 70-79 at the 1st Sep, and are not in an eligibility cohort.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>22. PNEUM Vacc given outwith age guidance</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - Pneumococcal vaccination records where the patient is under 65 years old at vaccination and not in an other eligibility cohort. Based on column S - age_at_vacc which is calculated using </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">column AC - patient_date_of_birth </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>and</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> column I - vacc_occurence_time</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>24. RSV Non-cohort vacc age&gt;55</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Records where the patient is aged over 55 and not in a vaccination eligibility cohort.</t>
     </r>
   </si>
 </sst>
@@ -1971,10 +2017,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E662A8FB-DAF5-4A29-98DF-C55E0C57EBEA}">
-  <dimension ref="B3:F37"/>
+  <dimension ref="B3:F39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2039,7 +2085,7 @@
       <c r="B9" s="1"/>
       <c r="C9" s="6"/>
       <c r="D9" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="1"/>
@@ -2073,7 +2119,7 @@
       <c r="B13" s="1"/>
       <c r="C13" s="6"/>
       <c r="D13" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="1"/>
@@ -2118,7 +2164,7 @@
       <c r="B18" s="1"/>
       <c r="C18" s="6"/>
       <c r="D18" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E18" s="7"/>
       <c r="F18" s="1"/>
@@ -2208,7 +2254,7 @@
       <c r="B28" s="1"/>
       <c r="C28" s="6"/>
       <c r="D28" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E28" s="7"/>
       <c r="F28" s="1"/>
@@ -2244,7 +2290,7 @@
       <c r="B32" s="1"/>
       <c r="C32" s="6"/>
       <c r="D32" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E32" s="7"/>
       <c r="F32" s="1"/>
@@ -2262,33 +2308,51 @@
       <c r="B34" s="1"/>
       <c r="C34" s="6"/>
       <c r="D34" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E34" s="7"/>
       <c r="F34" s="1"/>
     </row>
-    <row r="35" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B35" s="1"/>
       <c r="C35" s="6"/>
-      <c r="D35" s="8" t="s">
-        <v>43</v>
+      <c r="D35" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="E35" s="7"/>
       <c r="F35" s="1"/>
     </row>
-    <row r="36" spans="2:6" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B36" s="7"/>
-      <c r="C36" s="10"/>
-      <c r="D36" s="10"/>
-      <c r="E36" s="11"/>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B36" s="1"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E36" s="7"/>
       <c r="F36" s="1"/>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E37" s="7"/>
       <c r="F37" s="1"/>
+    </row>
+    <row r="38" spans="2:6" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B38" s="7"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="1"/>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update HB summary image with latest changes
</commit_message>
<xml_diff>
--- a/Scripts/Vacc HB DQ Summary template.xlsx
+++ b/Scripts/Vacc HB DQ Summary template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\nssstats01\VaccineDM\Mike\vacc-dq-reporting\Scripts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\nssstats01\VaccineDM\Mike\Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66F3756F-1739-42AF-B9B9-9856FB6D47CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D931037-9DEC-4603-B0CA-41BB8E92284D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="57">
   <si>
     <t>Notes on the report:</t>
   </si>
@@ -884,6 +884,180 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>06. COV Booster interval &lt; 12 weeks</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Covid-19 records where the patient has received a booster dose less than 12 weeks (84 days) after their previous vaccination.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>16. HZ Dose 2 interval &lt; 56 days</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Herpes zoster dose 2 records where the interval between dose 1 and dose 2 given is less than 56 days.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>01. Missing/Invalid CHI number</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Patients who have been recorded without a CHI number or with an invalid CHI number.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>20. HZ Vacc given outwith age guidance</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Herpes zoster vaccination records where, from 1st Sep 2023, the patient is not age 65 or 70-79 at 1st Sep 2023, or for previous years where a patient was not age 70-79 at the 1st Sep, and are not in an eligibility cohort.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>23. RSV Booster Recorded</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Records where a booster vaccination has been recorded.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>24. RSV Non-cohort vacc age&gt;55</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Records where the patient is aged over 55 and not in a vaccination eligibility cohort.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Column AI - patient_nrs_date_of_death</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is included but, due to inconsistencies with this data in the VDL, should only be used in conjunction with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>column AH - patient_chi_derived_status_desc</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> for assurance on whether a person has died.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>07. COV Under 12 adult dose</t>
     </r>
     <r>
@@ -926,7 +1100,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>column AC - patient_date_of_birth</t>
+      <t>column AD - patient_date_of_birth</t>
     </r>
     <r>
       <rPr>
@@ -1012,7 +1186,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>column AC - patient_date_of_birth</t>
+      <t>column AD - patient_date_of_birth</t>
     </r>
     <r>
       <rPr>
@@ -1090,7 +1264,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>column AC - patient_date_of_birth</t>
+      <t>column AD - patient_date_of_birth</t>
     </r>
     <r>
       <rPr>
@@ -1126,17 +1300,142 @@
   </si>
   <si>
     <r>
-      <t>14. FLU Fluenz age &lt;2, &gt;17</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - Flu records where the Fluenz vaccine has been given to patients aged under 2 or over 17. Based on </t>
+      <t>22. PNEUM Vacc given outwith age guidance</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Pneumococcal vaccination records where the patient is under 65 years old at vaccination and not in an other eligibility cohort. Based on column S - age_at_vacc which is calculated using </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">column AD - patient_date_of_birth </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>and</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> column I - vacc_occurence_time</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>25. COV Two or more boosters in campaign</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Covid-19 records from Spring 2024 programme onwards where the patient has received 2 or more booster doses in a single vaccination campaign/programme.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>26. COV Outwith vacc programme</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Covid-19 records from Spring 2024 programme onwards of vaccinations that have taken place outwith the advised dates of a vaccination programme.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>28. FLU AQIV given age &lt;50</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Flu records from Autumn/Winter 2024/25 programme onwards for AQIV products given to anyone under age 50.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>29. FLU Outwith Autumn/Winter campaigns</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Flu records from Autumn/Winter 2021/22 programme onwards of vaccinations that have taken place outwith the advised dates of a vaccination programme.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">14. FLU LAIV given age &lt;2 or &gt;18 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Flu records where an LAIV child vaccine has been given to patients aged under 2 or over 18. Based on </t>
     </r>
     <r>
       <rPr>
@@ -1168,7 +1467,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>column AC - patient_date_of_birth</t>
+      <t>column AD - patient_date_of_birth</t>
     </r>
     <r>
       <rPr>
@@ -1204,223 +1503,30 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Column AH - patient_nrs_date_of_death</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> is included but, due to inconsistencies with this data in the VDL, should only be used in conjunction with </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>column AG - patient_chi_derived_status_desc</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> for assurance on whether a person has died.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>06. COV Booster interval &lt; 12 weeks</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - Covid-19 records where the patient has received a booster dose less than 12 weeks (84 days) after their previous vaccination.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>16. HZ Dose 2 interval &lt; 56 days</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - Herpes zoster dose 2 records where the interval between dose 1 and dose 2 given is less than 56 days.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>01. Missing/Invalid CHI number</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - Patients who have been recorded without a CHI number or with an invalid CHI number.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>20. HZ Vacc given outwith age guidance</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - Herpes zoster vaccination records where, from 1st Sep 2023, the patient is not age 65 or 70-79 at 1st Sep 2023, or for previous years where a patient was not age 70-79 at the 1st Sep, and are not in an eligibility cohort.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>22. PNEUM Vacc given outwith age guidance</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - Pneumococcal vaccination records where the patient is under 65 years old at vaccination and not in an other eligibility cohort. Based on column S - age_at_vacc which is calculated using </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">column AC - patient_date_of_birth </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>and</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> column I - vacc_occurence_time</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>23. RSV Booster Recorded</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - Records where a booster vaccination has been recorded.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>25. All query data</t>
+      <t>27. COV Vacc given outwith age guidance</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Covid-19 records, from 1st April 2025, where the patient is not age 75 or over at 30th Jun 2025 and are not in an eligibility cohort.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>30. All query data</t>
     </r>
     <r>
       <rPr>
@@ -1494,29 +1600,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>, to see all data quality queries against them, rather than by query type.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>24. RSV Non-cohort vacc age&gt;55</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - Records where the patient is aged over 55 and not in a vaccination eligibility cohort.</t>
     </r>
   </si>
 </sst>
@@ -2017,10 +2100,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E662A8FB-DAF5-4A29-98DF-C55E0C57EBEA}">
-  <dimension ref="B3:F39"/>
+  <dimension ref="B3:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="B6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2085,7 +2168,7 @@
       <c r="B9" s="1"/>
       <c r="C9" s="6"/>
       <c r="D9" s="8" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="1"/>
@@ -2119,7 +2202,7 @@
       <c r="B13" s="1"/>
       <c r="C13" s="6"/>
       <c r="D13" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="1"/>
@@ -2164,7 +2247,7 @@
       <c r="B18" s="1"/>
       <c r="C18" s="6"/>
       <c r="D18" s="8" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E18" s="7"/>
       <c r="F18" s="1"/>
@@ -2173,7 +2256,7 @@
       <c r="B19" s="1"/>
       <c r="C19" s="6"/>
       <c r="D19" s="8" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="1"/>
@@ -2182,7 +2265,7 @@
       <c r="B20" s="1"/>
       <c r="C20" s="6"/>
       <c r="D20" s="8" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="1"/>
@@ -2191,7 +2274,7 @@
       <c r="B21" s="8"/>
       <c r="C21" s="16"/>
       <c r="D21" s="17" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="E21" s="18"/>
       <c r="F21" s="8"/>
@@ -2236,7 +2319,7 @@
       <c r="B26" s="1"/>
       <c r="C26" s="6"/>
       <c r="D26" s="17" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E26" s="7"/>
       <c r="F26" s="1"/>
@@ -2254,7 +2337,7 @@
       <c r="B28" s="1"/>
       <c r="C28" s="6"/>
       <c r="D28" s="8" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E28" s="7"/>
       <c r="F28" s="1"/>
@@ -2290,7 +2373,7 @@
       <c r="B32" s="1"/>
       <c r="C32" s="6"/>
       <c r="D32" s="17" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E32" s="7"/>
       <c r="F32" s="1"/>
@@ -2308,7 +2391,7 @@
       <c r="B34" s="1"/>
       <c r="C34" s="6"/>
       <c r="D34" s="17" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E34" s="7"/>
       <c r="F34" s="1"/>
@@ -2317,7 +2400,7 @@
       <c r="B35" s="1"/>
       <c r="C35" s="6"/>
       <c r="D35" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E35" s="7"/>
       <c r="F35" s="1"/>
@@ -2326,7 +2409,7 @@
       <c r="B36" s="1"/>
       <c r="C36" s="6"/>
       <c r="D36" s="1" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="E36" s="7"/>
       <c r="F36" s="1"/>
@@ -2334,25 +2417,70 @@
     <row r="37" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B37" s="1"/>
       <c r="C37" s="6"/>
-      <c r="D37" s="8" t="s">
+      <c r="D37" s="17" t="s">
         <v>50</v>
       </c>
       <c r="E37" s="7"/>
       <c r="F37" s="1"/>
     </row>
-    <row r="38" spans="2:6" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B38" s="7"/>
-      <c r="C38" s="10"/>
-      <c r="D38" s="10"/>
-      <c r="E38" s="11"/>
+    <row r="38" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="B38" s="1"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E38" s="7"/>
       <c r="F38" s="1"/>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="E39" s="7"/>
       <c r="F39" s="1"/>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B40" s="1"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="E40" s="7"/>
+      <c r="F40" s="1"/>
+    </row>
+    <row r="41" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="B41" s="1"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="E41" s="7"/>
+      <c r="F41" s="1"/>
+    </row>
+    <row r="42" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="B42" s="1"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E42" s="7"/>
+      <c r="F42" s="1"/>
+    </row>
+    <row r="43" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B43" s="7"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="11"/>
+      <c r="F43" s="1"/>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
in main DQ script - update code for HZ eligibility query to use age at 01sep instead of DOBs, and update script for 2025-26. Also update DQ report summary details in template and image for HZ age eligibility query.
</commit_message>
<xml_diff>
--- a/Scripts/Vacc HB DQ Summary template.xlsx
+++ b/Scripts/Vacc HB DQ Summary template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\nssstats01\VaccineDM\Mike\Scripts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\stats\VaccineDM\Mike\Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D931037-9DEC-4603-B0CA-41BB8E92284D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54848327-2932-497E-A916-CE242811B5ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary Notes 1 (2)" sheetId="3" r:id="rId1"/>
@@ -945,6 +945,650 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>23. RSV Booster Recorded</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Records where a booster vaccination has been recorded.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>24. RSV Non-cohort vacc age&gt;55</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Records where the patient is aged over 55 and not in a vaccination eligibility cohort.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Column AI - patient_nrs_date_of_death</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is included but, due to inconsistencies with this data in the VDL, should only be used in conjunction with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>column AH - patient_chi_derived_status_desc</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> for assurance on whether a person has died.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>07. COV Under 12 adult dose</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Covid-19 records of patients aged under 12 at vaccination who have received a full dose of a vaccine. Based on c</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>olumn S - age_at_vacc</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> which is calculated using </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>column AD - patient_date_of_birth</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>column I - vacc_occurence_time</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>08. COV Over 11 or under 5 paediatric dose</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Covid-19 records of patients aged over 11 or under 5 at vaccination who have received a paediatric dose. Based on </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>column S - age_at_vacc</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> which is calculated using </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>column AD - patient_date_of_birth</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>column I - vacc_occurence_time</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>09. COV Over 4 infant dose</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Covid records of patients aged over 4 at vaccination who have received an infant dose. Based on </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>column S - age_at_vacc</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> which is calculated using </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>column AD - patient_date_of_birth</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>column I - vacc_occurence_time</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>22. PNEUM Vacc given outwith age guidance</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Pneumococcal vaccination records where the patient is under 65 years old at vaccination and not in an other eligibility cohort. Based on column S - age_at_vacc which is calculated using </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">column AD - patient_date_of_birth </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>and</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> column I - vacc_occurence_time</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>25. COV Two or more boosters in campaign</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Covid-19 records from Spring 2024 programme onwards where the patient has received 2 or more booster doses in a single vaccination campaign/programme.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>26. COV Outwith vacc programme</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Covid-19 records from Spring 2024 programme onwards of vaccinations that have taken place outwith the advised dates of a vaccination programme.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>28. FLU AQIV given age &lt;50</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Flu records from Autumn/Winter 2024/25 programme onwards for AQIV products given to anyone under age 50.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>29. FLU Outwith Autumn/Winter campaigns</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Flu records from Autumn/Winter 2021/22 programme onwards of vaccinations that have taken place outwith the advised dates of a vaccination programme.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">14. FLU LAIV given age &lt;2 or &gt;18 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Flu records where an LAIV child vaccine has been given to patients aged under 2 or over 18. Based on </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>column S - age_at_vacc</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> which is calculated using </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>column AD - patient_date_of_birth</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>column I - vacc_occurence_time</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>27. COV Vacc given outwith age guidance</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Covid-19 records, from 1st April 2025, where the patient is not age 75 or over at 30th Jun 2025 and are not in an eligibility cohort.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>30. All query data</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - All records that appear in the above queries. (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>QueryType</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is listed in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>column A</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">.) This can be used to focus on individual patients by filtering by </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>column D - patient_derived_upi_number</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, to see all data quality queries against them, rather than by query type.</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t>20. HZ Vacc given outwith age guidance</t>
     </r>
     <r>
@@ -955,651 +1599,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> - Herpes zoster vaccination records where, from 1st Sep 2023, the patient is not age 65 or 70-79 at 1st Sep 2023, or for previous years where a patient was not age 70-79 at the 1st Sep, and are not in an eligibility cohort.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>23. RSV Booster Recorded</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - Records where a booster vaccination has been recorded.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>24. RSV Non-cohort vacc age&gt;55</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - Records where the patient is aged over 55 and not in a vaccination eligibility cohort.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Column AI - patient_nrs_date_of_death</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> is included but, due to inconsistencies with this data in the VDL, should only be used in conjunction with </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>column AH - patient_chi_derived_status_desc</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> for assurance on whether a person has died.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>07. COV Under 12 adult dose</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - Covid-19 records of patients aged under 12 at vaccination who have received a full dose of a vaccine. Based on c</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>olumn S - age_at_vacc</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> which is calculated using </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>column AD - patient_date_of_birth</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> and </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>column I - vacc_occurence_time</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>08. COV Over 11 or under 5 paediatric dose</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - Covid-19 records of patients aged over 11 or under 5 at vaccination who have received a paediatric dose. Based on </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>column S - age_at_vacc</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> which is calculated using </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>column AD - patient_date_of_birth</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> and </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>column I - vacc_occurence_time</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>09. COV Over 4 infant dose</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - Covid records of patients aged over 4 at vaccination who have received an infant dose. Based on </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>column S - age_at_vacc</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> which is calculated using </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>column AD - patient_date_of_birth</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> and </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>column I - vacc_occurence_time</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>22. PNEUM Vacc given outwith age guidance</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - Pneumococcal vaccination records where the patient is under 65 years old at vaccination and not in an other eligibility cohort. Based on column S - age_at_vacc which is calculated using </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">column AD - patient_date_of_birth </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>and</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> column I - vacc_occurence_time</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>25. COV Two or more boosters in campaign</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - Covid-19 records from Spring 2024 programme onwards where the patient has received 2 or more booster doses in a single vaccination campaign/programme.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>26. COV Outwith vacc programme</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - Covid-19 records from Spring 2024 programme onwards of vaccinations that have taken place outwith the advised dates of a vaccination programme.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>28. FLU AQIV given age &lt;50</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - Flu records from Autumn/Winter 2024/25 programme onwards for AQIV products given to anyone under age 50.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>29. FLU Outwith Autumn/Winter campaigns</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - Flu records from Autumn/Winter 2021/22 programme onwards of vaccinations that have taken place outwith the advised dates of a vaccination programme.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">14. FLU LAIV given age &lt;2 or &gt;18 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - Flu records where an LAIV child vaccine has been given to patients aged under 2 or over 18. Based on </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>column S - age_at_vacc</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> which is calculated using </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>column AD - patient_date_of_birth</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> and </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>column I - vacc_occurence_time</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>27. COV Vacc given outwith age guidance</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - Covid-19 records, from 1st April 2025, where the patient is not age 75 or over at 30th Jun 2025 and are not in an eligibility cohort.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>30. All query data</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - All records that appear in the above queries. (</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>QueryType</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> is listed in </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>column A</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">.) This can be used to focus on individual patients by filtering by </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>column D - patient_derived_upi_number</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, to see all data quality queries against them, rather than by query type.</t>
+      <t xml:space="preserve"> - Herpes zoster vaccination records where the patient is not of eligible age at 1st Sep of that year and are not in any other eligibility cohort.</t>
     </r>
   </si>
 </sst>
@@ -2102,8 +2102,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E662A8FB-DAF5-4A29-98DF-C55E0C57EBEA}">
   <dimension ref="B3:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2168,7 +2168,7 @@
       <c r="B9" s="1"/>
       <c r="C9" s="6"/>
       <c r="D9" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="1"/>
@@ -2256,7 +2256,7 @@
       <c r="B19" s="1"/>
       <c r="C19" s="6"/>
       <c r="D19" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="1"/>
@@ -2265,7 +2265,7 @@
       <c r="B20" s="1"/>
       <c r="C20" s="6"/>
       <c r="D20" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="1"/>
@@ -2274,7 +2274,7 @@
       <c r="B21" s="8"/>
       <c r="C21" s="16"/>
       <c r="D21" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E21" s="18"/>
       <c r="F21" s="8"/>
@@ -2319,7 +2319,7 @@
       <c r="B26" s="1"/>
       <c r="C26" s="6"/>
       <c r="D26" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E26" s="7"/>
       <c r="F26" s="1"/>
@@ -2373,7 +2373,7 @@
       <c r="B32" s="1"/>
       <c r="C32" s="6"/>
       <c r="D32" s="17" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="E32" s="7"/>
       <c r="F32" s="1"/>
@@ -2391,7 +2391,7 @@
       <c r="B34" s="1"/>
       <c r="C34" s="6"/>
       <c r="D34" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E34" s="7"/>
       <c r="F34" s="1"/>
@@ -2400,7 +2400,7 @@
       <c r="B35" s="1"/>
       <c r="C35" s="6"/>
       <c r="D35" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E35" s="7"/>
       <c r="F35" s="1"/>
@@ -2409,7 +2409,7 @@
       <c r="B36" s="1"/>
       <c r="C36" s="6"/>
       <c r="D36" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E36" s="7"/>
       <c r="F36" s="1"/>
@@ -2418,7 +2418,7 @@
       <c r="B37" s="1"/>
       <c r="C37" s="6"/>
       <c r="D37" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E37" s="7"/>
       <c r="F37" s="1"/>
@@ -2427,7 +2427,7 @@
       <c r="B38" s="1"/>
       <c r="C38" s="6"/>
       <c r="D38" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E38" s="7"/>
       <c r="F38" s="1"/>
@@ -2436,7 +2436,7 @@
       <c r="B39" s="1"/>
       <c r="C39" s="6"/>
       <c r="D39" s="17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E39" s="7"/>
       <c r="F39" s="1"/>
@@ -2445,7 +2445,7 @@
       <c r="B40" s="1"/>
       <c r="C40" s="6"/>
       <c r="D40" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E40" s="7"/>
       <c r="F40" s="1"/>
@@ -2454,7 +2454,7 @@
       <c r="B41" s="1"/>
       <c r="C41" s="6"/>
       <c r="D41" s="17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E41" s="7"/>
       <c r="F41" s="1"/>
@@ -2463,7 +2463,7 @@
       <c r="B42" s="1"/>
       <c r="C42" s="6"/>
       <c r="D42" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E42" s="7"/>
       <c r="F42" s="1"/>
@@ -2725,4 +2725,10 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{b4199b9c-a89e-442f-9799-431511f14748}" enabled="1" method="Privileged" siteId="{10efe0bd-a030-4bca-809c-b5e6745e499a}" contentBits="0" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>